<commit_message>
Switch to 2 asset class Ivy Portfolio
</commit_message>
<xml_diff>
--- a/Historical Prices/Portfolio.xlsx
+++ b/Historical Prices/Portfolio.xlsx
@@ -8,24 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s1614973_ed_ac_uk/Documents/Every Day Files/Documents/Finance/Ivy Portfolio/Historical Prices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="11_F25DC773A252ABDACC104897791A755A5BDE58EC" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8166C429-1FDD-4415-BE8E-A8DFAA1A80CC}"/>
+  <xr:revisionPtr revIDLastSave="306" documentId="11_F25DC773A252ABDACC104897791A755A5BDE58EC" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7FF23E2B-0DF2-43E2-B3B6-DB84F4622749}"/>
   <bookViews>
-    <workbookView xWindow="3750" yWindow="3225" windowWidth="24810" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ivy Constituents" sheetId="1" r:id="rId1"/>
+    <sheet name="Ivy Decision" sheetId="2" r:id="rId2"/>
+    <sheet name="Ivy Action" sheetId="3" r:id="rId3"/>
+    <sheet name="Mutual Constituents" sheetId="4" r:id="rId4"/>
+    <sheet name="Mutual Action" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
   <si>
     <t>Fund</t>
   </si>
@@ -109,14 +121,118 @@
   </si>
   <si>
     <t>GB00B99BDY18</t>
+  </si>
+  <si>
+    <t>200 day SMA</t>
+  </si>
+  <si>
+    <t>3 months</t>
+  </si>
+  <si>
+    <t>6 months</t>
+  </si>
+  <si>
+    <t>12 months</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Below</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Above</t>
+  </si>
+  <si>
+    <t>Portfolio Value</t>
+  </si>
+  <si>
+    <t>Cash Added</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>First Amount</t>
+  </si>
+  <si>
+    <t>Second Amount</t>
+  </si>
+  <si>
+    <t>Held as Cash</t>
+  </si>
+  <si>
+    <t>FUNDSMITH EQUITY</t>
+  </si>
+  <si>
+    <t>GB00B41YBW71</t>
+  </si>
+  <si>
+    <t>LEGAL &amp; GENERAL GLOBAL TECHNOLOGY INDEX</t>
+  </si>
+  <si>
+    <t>GB00B0CNH163</t>
+  </si>
+  <si>
+    <t>LF LINDSELL TRAIN UK EQUITY</t>
+  </si>
+  <si>
+    <t>GB00BJFLM156</t>
+  </si>
+  <si>
+    <t>LINDSELL TRAIN GLOBAL EQUITY</t>
+  </si>
+  <si>
+    <t>IE00BJSPMJ28</t>
+  </si>
+  <si>
+    <t>MARLBOROUGH UK MICRO-CAP GROWTH</t>
+  </si>
+  <si>
+    <t>GB00B8F8YX59</t>
+  </si>
+  <si>
+    <t>Fundsmith</t>
+  </si>
+  <si>
+    <t>International Index</t>
+  </si>
+  <si>
+    <t>Global Technology Index</t>
+  </si>
+  <si>
+    <t>Lindsell Train UK</t>
+  </si>
+  <si>
+    <t>Lindsell Train Global</t>
+  </si>
+  <si>
+    <t>Marlborough UK Micro Cap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -132,7 +248,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -140,12 +256,99 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,4 +744,873 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F4D358C-AB38-4A28-8D96-7E4BC2E5DB20}">
+  <dimension ref="B2:AA39"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" customWidth="1"/>
+    <col min="18" max="18" width="12" customWidth="1"/>
+    <col min="23" max="23" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="C2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="11"/>
+      <c r="AA2" s="11"/>
+    </row>
+    <row r="3" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="W3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="X3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA3" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
+        <v>43893</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="4">
+        <v>-0.1845</v>
+      </c>
+      <c r="E4" s="4">
+        <v>-0.13539999999999999</v>
+      </c>
+      <c r="F4" s="4">
+        <v>-8.1299999999999997E-2</v>
+      </c>
+      <c r="G4" s="5">
+        <f>AVERAGE(D4:F4)</f>
+        <v>-0.13373333333333332</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="4">
+        <v>-0.28039999999999998</v>
+      </c>
+      <c r="J4" s="4">
+        <v>-0.2243</v>
+      </c>
+      <c r="K4" s="4">
+        <v>-0.23169999999999999</v>
+      </c>
+      <c r="L4" s="5">
+        <f>AVERAGE(I4:K4)</f>
+        <v>-0.24546666666666664</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" s="4">
+        <v>-0.29170000000000001</v>
+      </c>
+      <c r="O4" s="4">
+        <v>-0.32319999999999999</v>
+      </c>
+      <c r="P4" s="4">
+        <v>-0.25190000000000001</v>
+      </c>
+      <c r="Q4" s="5">
+        <f>AVERAGE(N4:P4)</f>
+        <v>-0.28893333333333332</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4" s="4">
+        <v>-0.1017</v>
+      </c>
+      <c r="T4" s="4">
+        <v>-9.5000000000000001E-2</v>
+      </c>
+      <c r="U4" s="4">
+        <v>0.1704</v>
+      </c>
+      <c r="V4" s="5">
+        <f>AVERAGE(S4:U4)</f>
+        <v>-8.7666666666666639E-3</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="X4" s="4">
+        <v>5.3900000000000003E-2</v>
+      </c>
+      <c r="Y4" s="4">
+        <v>2.4199999999999999E-2</v>
+      </c>
+      <c r="Z4" s="4">
+        <v>0.1082</v>
+      </c>
+      <c r="AA4" s="5">
+        <f>AVERAGE(X4:Z4)</f>
+        <v>6.2100000000000009E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B5" s="8"/>
+      <c r="C5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+      <c r="C7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+      <c r="C8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="Q8" s="1"/>
+    </row>
+    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+      <c r="C9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="Q9" s="1"/>
+    </row>
+    <row r="10" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+      <c r="C10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="Q10" s="1"/>
+    </row>
+    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+      <c r="C11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="Q11" s="1"/>
+    </row>
+    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+      <c r="C12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
+      <c r="C13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="Q13" s="1"/>
+    </row>
+    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B14" s="8"/>
+      <c r="C14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="Q14" s="1"/>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B15" s="8"/>
+      <c r="C15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="Q15" s="1"/>
+    </row>
+    <row r="16" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B16" s="8"/>
+      <c r="C16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B17" s="8"/>
+      <c r="C17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="Q17" s="1"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B18" s="8"/>
+      <c r="C18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="Q18" s="1"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B19" s="8"/>
+      <c r="C19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="Q19" s="1"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B20" s="8"/>
+      <c r="C20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="Q20" s="1"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B21" s="8"/>
+      <c r="C21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="Q21" s="1"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B22" s="8"/>
+      <c r="C22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="Q22" s="1"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B23" s="8"/>
+      <c r="C23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="Q23" s="1"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B24" s="8"/>
+      <c r="C24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="Q24" s="1"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B25" s="8"/>
+      <c r="C25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="Q25" s="1"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B26" s="8"/>
+      <c r="C26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="Q26" s="1"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B27" s="8"/>
+      <c r="C27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="Q27" s="1"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B28" s="8"/>
+      <c r="C28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="Q28" s="1"/>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B29" s="8"/>
+      <c r="C29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="Q29" s="1"/>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B30" s="8"/>
+      <c r="C30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="Q30" s="1"/>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B31" s="8"/>
+      <c r="C31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B32" s="8"/>
+      <c r="C32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="L32" s="1"/>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="8"/>
+      <c r="C33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="L33" s="1"/>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="8"/>
+      <c r="C34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="L34" s="1"/>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="8"/>
+      <c r="C35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="8"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="8"/>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="8"/>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="W2:AA2"/>
+    <mergeCell ref="R2:V2"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="M2:Q2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37DCA578-1F87-4976-AF4B-D83082AB3C25}">
+  <dimension ref="B3:I39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
+        <v>43893</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9">
+        <v>3500</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="9">
+        <f>D4/2</f>
+        <v>1750</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0</v>
+      </c>
+      <c r="I4" s="9">
+        <f>C4+D4-F4-H4</f>
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="8"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="8"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="8"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="8"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="8"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="8"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="8"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="8"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="8"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="8"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="8"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="8"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="8"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="8"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="8"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="8"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="8"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="8"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="8"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="8"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="8"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="8"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="8"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="8"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="8"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="8"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="8"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="8"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="8"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="8"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="8"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B37A92EA-DCC9-4488-A72A-78562D9446DB}">
+  <dimension ref="B2:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="44.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57614DF7-7126-4BC8-8BF5-3337780A019D}">
+  <dimension ref="B2:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="7" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" customWidth="1"/>
+    <col min="10" max="10" width="25.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="6">
+        <v>43893</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9">
+        <v>3500</v>
+      </c>
+      <c r="E3" s="9">
+        <v>0</v>
+      </c>
+      <c r="F3" s="9">
+        <v>0</v>
+      </c>
+      <c r="G3" s="9">
+        <v>0</v>
+      </c>
+      <c r="H3" s="9">
+        <v>0</v>
+      </c>
+      <c r="I3" s="9">
+        <v>0</v>
+      </c>
+      <c r="J3" s="9">
+        <v>0</v>
+      </c>
+      <c r="K3" s="9">
+        <f>SUM(C3:D3)-SUM(E3:J3)</f>
+        <v>3500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed bug where 3, 6, and 12 month returns were calculated wrong. Made it so weekends are excluded
</commit_message>
<xml_diff>
--- a/Historical Prices/Portfolio.xlsx
+++ b/Historical Prices/Portfolio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiera\OneDrive - University of Edinburgh\Every Day Files\Documents\Finance\Ivy Portfolio\Historical Prices\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s1614973_ed_ac_uk/Documents/Every Day Files/Documents/Finance/Ivy Portfolio/Historical Prices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6089D76E-BD2A-4ED7-9A08-2E6867C7FAC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{B3655B11-2F62-4153-BCBA-894DDAAB8C62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1425" yWindow="1425" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constiuents" sheetId="1" r:id="rId1"/>

</xml_diff>